<commit_message>
fine alberatura tcr - fcf
</commit_message>
<xml_diff>
--- a/FCF/Configurazioni/Configurazione_Start_Run.xlsx
+++ b/FCF/Configurazioni/Configurazione_Start_Run.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://picinformaticait-my.sharepoint.com/personal/mmenchicchi_pic-informatica_it1/Documents/Condivisione ENI PIC/NDP/RFCF/file esterni/fcf1/configurazione_start_run/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\file_caricamento\FCF\Configurazioni\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_AD4D5CB4E552A5DACE1C647C80184BC65BDEDD88" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{799516F5-0333-453C-BC21-5B81F6A7B253}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F73A1120-6ABE-48C6-8F13-42DBCD3C87F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>id_run_fw</t>
   </si>
@@ -61,6 +61,18 @@
   </si>
   <si>
     <t>EMISSIONE</t>
+  </si>
+  <si>
+    <t>-- se calcoliamo un anno solo forecast: mettere mese_fine_cons e max_emissione_cons a 0</t>
+  </si>
+  <si>
+    <t>-- se non vogliamo calcolare rateo anni precedenti, inserire 00000000 sotto ds_ric_gas_anno_prec e ds_ric_pwr_anno_prec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-- anno_prec_tipologia = DELTA o anno_prec_tipologia = EMISSIONE -&gt; modalità di calcolo del rateo anni precedenti (utile nel BUDGET fatto a ottobre/novembre sull'anno successivo) </t>
+  </si>
+  <si>
+    <t>GUIDA</t>
   </si>
 </sst>
 </file>
@@ -387,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -406,7 +418,7 @@
     <col min="10" max="10" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -437,8 +449,11 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="O1" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>26</v>
       </c>
@@ -468,6 +483,19 @@
       </c>
       <c r="J2" t="s">
         <v>11</v>
+      </c>
+      <c r="O2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O4" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correzione colonna data reperforming in flag reperforming
</commit_message>
<xml_diff>
--- a/FCF/Configurazioni/Configurazione_Start_Run.xlsx
+++ b/FCF/Configurazioni/Configurazione_Start_Run.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dbasilico\Desktop\file_caricamento\FCF\Configurazioni\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E48A111-BFCB-47A0-81E9-EF3B9A760092}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09CC402F-2053-45B6-A8AC-8CCA1D0A0E4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25695" yWindow="1230" windowWidth="23760" windowHeight="13230" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28260" yWindow="1470" windowWidth="24570" windowHeight="13230" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>id_run_fw</t>
   </si>
@@ -75,7 +75,10 @@
     <t>GUIDA</t>
   </si>
   <si>
-    <t>data_reperforming</t>
+    <t>flag_reperforming</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -405,7 +408,7 @@
   <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -491,6 +494,9 @@
       <c r="J2" t="s">
         <v>11</v>
       </c>
+      <c r="K2" t="s">
+        <v>17</v>
+      </c>
       <c r="O2" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
correzione flag_storicizzazione in data_forzatura_storico
</commit_message>
<xml_diff>
--- a/FCF/Configurazioni/Configurazione_Start_Run.xlsx
+++ b/FCF/Configurazioni/Configurazione_Start_Run.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dbasilico\Desktop\file_caricamento\FCF\Configurazioni\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09CC402F-2053-45B6-A8AC-8CCA1D0A0E4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ECFB029-8141-4039-8D0D-041932643BC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28260" yWindow="1470" windowWidth="24570" windowHeight="13230" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2016" yWindow="1716" windowWidth="33312" windowHeight="14220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>id_run_fw</t>
   </si>
@@ -75,10 +75,25 @@
     <t>GUIDA</t>
   </si>
   <si>
-    <t>flag_reperforming</t>
-  </si>
-  <si>
-    <t>N</t>
+    <t>data_forzatura_storico</t>
+  </si>
+  <si>
+    <t>NOTE data_forzatura_storico</t>
+  </si>
+  <si>
+    <t>certa data (run reperforming)</t>
+  </si>
+  <si>
+    <t>se non valorizzata vengono prese le ultime anagrafiche presenti</t>
+  </si>
+  <si>
+    <t>FORMATO DATA: yyyy-mm-dd HH:mm:ss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data utilizzata per forzare il recupero delle tabelle delle anagrafiche strettamente minori di una </t>
+  </si>
+  <si>
+    <t>2022-10-24 10:43:21</t>
   </si>
 </sst>
 </file>
@@ -122,9 +137,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -405,9 +422,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
@@ -422,7 +439,8 @@
     <col min="8" max="8" width="21.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28" style="3" customWidth="1"/>
+    <col min="12" max="12" width="20.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
@@ -456,7 +474,7 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>16</v>
       </c>
       <c r="O1" s="1" t="s">
@@ -494,8 +512,8 @@
       <c r="J2" t="s">
         <v>11</v>
       </c>
-      <c r="K2" t="s">
-        <v>17</v>
+      <c r="K2" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="O2" t="s">
         <v>12</v>
@@ -509,6 +527,31 @@
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="O4" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O6" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O10" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correzione configurazione start run RFCF1
</commit_message>
<xml_diff>
--- a/FCF/Configurazioni/Configurazione_Start_Run.xlsx
+++ b/FCF/Configurazioni/Configurazione_Start_Run.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dbasilico\Desktop\file_caricamento\FCF\Configurazioni\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ECFB029-8141-4039-8D0D-041932643BC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98531638-EB0E-48A0-87DA-C91E828D3D4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2016" yWindow="1716" windowWidth="33312" windowHeight="14220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2016" yWindow="1716" windowWidth="16776" windowHeight="14220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -424,8 +424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Data forzatura storico posta a none
</commit_message>
<xml_diff>
--- a/FCF/Configurazioni/Configurazione_Start_Run.xlsx
+++ b/FCF/Configurazioni/Configurazione_Start_Run.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dbasilico\Desktop\file_caricamento\FCF\Configurazioni\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98531638-EB0E-48A0-87DA-C91E828D3D4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45EF6362-9DBF-419D-8DA6-B7FB1D2D97ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2016" yWindow="1716" windowWidth="16776" windowHeight="14220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2016" yWindow="1716" windowWidth="27348" windowHeight="14220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>id_run_fw</t>
   </si>
@@ -91,9 +91,6 @@
   </si>
   <si>
     <t xml:space="preserve">data utilizzata per forzare il recupero delle tabelle delle anagrafiche strettamente minori di una </t>
-  </si>
-  <si>
-    <t>2022-10-24 10:43:21</t>
   </si>
 </sst>
 </file>
@@ -425,7 +422,7 @@
   <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -512,9 +509,6 @@
       <c r="J2" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="O2" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
Cambio formato ds_ric_gas/pwe_anno_prec config start run
</commit_message>
<xml_diff>
--- a/FCF/Configurazioni/Configurazione_Start_Run.xlsx
+++ b/FCF/Configurazioni/Configurazione_Start_Run.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dbasilico\Desktop\file_caricamento\FCF\Configurazioni\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45EF6362-9DBF-419D-8DA6-B7FB1D2D97ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C730AA3C-0285-4A11-B346-9B1BF000DAED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2016" yWindow="1716" windowWidth="27348" windowHeight="14220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3012" yWindow="504" windowWidth="23520" windowHeight="14220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>id_run_fw</t>
   </si>
@@ -91,6 +91,15 @@
   </si>
   <si>
     <t xml:space="preserve">data utilizzata per forzare il recupero delle tabelle delle anagrafiche strettamente minori di una </t>
+  </si>
+  <si>
+    <t>NOTE ric_anno_prec_gas/pwr</t>
+  </si>
+  <si>
+    <t>2022-02-24 00:00:00</t>
+  </si>
+  <si>
+    <t>inserire data snapshot da estrarre in preparazione_dati_inigestion</t>
   </si>
 </sst>
 </file>
@@ -419,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -432,8 +441,9 @@
     <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.109375" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19.88671875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="28" style="3" customWidth="1"/>
@@ -459,10 +469,10 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -497,11 +507,11 @@
       <c r="F2">
         <v>5</v>
       </c>
-      <c r="G2">
-        <v>20220224</v>
-      </c>
-      <c r="H2">
-        <v>20220224</v>
+      <c r="G2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="I2" t="s">
         <v>10</v>
@@ -545,6 +555,21 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="O10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O12" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O14" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Correzione anno_inizio e fine config start run RFCF_fatt
</commit_message>
<xml_diff>
--- a/FCF/Configurazioni/Configurazione_Start_Run.xlsx
+++ b/FCF/Configurazioni/Configurazione_Start_Run.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dbasilico\Desktop\file_caricamento\FCF\Configurazioni\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D329692-5A22-44D6-86F3-08CC4402307E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3134F089-6B15-4384-ADBA-0EA22187E1A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7080" yWindow="1980" windowWidth="22644" windowHeight="14220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2844" yWindow="1236" windowWidth="33408" windowHeight="14220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -431,7 +431,7 @@
   <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -493,10 +493,10 @@
         <v>26</v>
       </c>
       <c r="B2">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C2">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="D2">
         <v>117</v>

</xml_diff>

<commit_message>
Correzione configurazione start_run (anno inizio e fine 2021)
</commit_message>
<xml_diff>
--- a/FCF/Configurazioni/Configurazione_Start_Run.xlsx
+++ b/FCF/Configurazioni/Configurazione_Start_Run.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dbasilico\Desktop\file_caricamento\FCF\Configurazioni\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3134F089-6B15-4384-ADBA-0EA22187E1A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9868DD5F-0ABA-4112-8C59-95F2C6EC5543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2844" yWindow="1236" windowWidth="33408" windowHeight="14220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="48" yWindow="804" windowWidth="30024" windowHeight="14220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
   <si>
     <t>id_run_fw</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>inserire data snapshot da estrarre in preparazione_dati_inigestion</t>
+  </si>
+  <si>
+    <t>2021</t>
   </si>
 </sst>
 </file>
@@ -143,9 +146,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -431,23 +433,23 @@
   <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28" style="3" customWidth="1"/>
-    <col min="12" max="12" width="20.109375" customWidth="1"/>
+    <col min="1" max="1" width="10" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="20.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28" style="2" customWidth="1"/>
+    <col min="12" max="12" width="20.109375" style="2" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
@@ -469,10 +471,10 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -481,7 +483,7 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="O1" s="1" t="s">
@@ -489,47 +491,47 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="A2" s="2">
         <v>26</v>
       </c>
-      <c r="B2">
-        <v>2022</v>
-      </c>
-      <c r="C2">
-        <v>2022</v>
-      </c>
-      <c r="D2">
+      <c r="B2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="2">
         <v>117</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <v>5</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="2">
         <v>5</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O2" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="O3" t="s">
+      <c r="O3" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="O4" t="s">
+      <c r="O4" s="2" t="s">
         <v>14</v>
       </c>
     </row>
@@ -539,22 +541,22 @@
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="O7" t="s">
+      <c r="O7" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="O8" t="s">
+      <c r="O8" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="O9" t="s">
+      <c r="O9" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="O10" t="s">
+      <c r="O10" s="2" t="s">
         <v>20</v>
       </c>
     </row>
@@ -564,12 +566,12 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="O13" t="s">
+      <c r="O13" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="O14" t="s">
+      <c r="O14" s="2" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>